<commit_message>
search priority by table
</commit_message>
<xml_diff>
--- a/Shedule/Shedule/example.xlsx
+++ b/Shedule/Shedule/example.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28919"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28928"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D26F6C05-5E22-4786-B930-1A21016E8E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9CD74E7-87E3-42A4-9CCB-1046C7154158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +32,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+  <si>
+    <t>,vp[av</t>
+  </si>
+  <si>
+    <t>avdf</t>
+  </si>
+  <si>
+    <t>dfvfdv</t>
+  </si>
+  <si>
+    <t>avddfv</t>
+  </si>
   <si>
     <t>имя</t>
   </si>
@@ -54,22 +67,25 @@
     <t>степан</t>
   </si>
   <si>
+    <t>информатика, математика,физика</t>
+  </si>
+  <si>
+    <t>кирилл</t>
+  </si>
+  <si>
+    <t>математика, информатика</t>
+  </si>
+  <si>
+    <t>александр</t>
+  </si>
+  <si>
+    <t>физика, информатика, математика</t>
+  </si>
+  <si>
+    <t>вадим</t>
+  </si>
+  <si>
     <t>информатика, математика</t>
-  </si>
-  <si>
-    <t>кирилл</t>
-  </si>
-  <si>
-    <t>математика, информатика</t>
-  </si>
-  <si>
-    <t>александр</t>
-  </si>
-  <si>
-    <t>физика, информатика, математика</t>
-  </si>
-  <si>
-    <t>вадим</t>
   </si>
   <si>
     <t>ученик</t>
@@ -471,11 +487,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9AECF6-6A13-4C06-968C-F4509D45D703}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -489,30 +536,30 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1">
         <v>0.41666666666666669</v>
@@ -521,18 +568,18 @@
         <v>0.625</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1">
         <v>0.41666666666666669</v>
@@ -541,18 +588,18 @@
         <v>0.625</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1">
         <v>0.41666666666666669</v>
@@ -561,18 +608,18 @@
         <v>0.625</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1">
         <v>0.41666666666666669</v>
@@ -586,13 +633,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1">
         <v>0.41666666666666669</v>
@@ -603,10 +650,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="B8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1">
         <v>0.41666666666666669</v>
@@ -617,10 +664,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="B9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1">
         <v>0.41666666666666669</v>
@@ -631,10 +678,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="B10" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1">
         <v>0.41666666666666669</v>
@@ -645,10 +692,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="B11" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1">
         <v>0.41666666666666669</v>
@@ -659,10 +706,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="B12" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1">
         <v>0.41666666666666669</v>

</xml_diff>

<commit_message>
start of transition to time slots
</commit_message>
<xml_diff>
--- a/Shedule/Shedule/example.xlsx
+++ b/Shedule/Shedule/example.xlsx
@@ -16,7 +16,7 @@
     <x:sheet name="преподы" sheetId="2" r:id="rId1"/>
     <x:sheet name="ученики" sheetId="1" r:id="rId2"/>
     <x:sheet name="квалификации" sheetId="3" r:id="rId3"/>
-    <x:sheet name="Расписание и комбинации" sheetId="40" r:id="rId8"/>
+    <x:sheet name="Расписание и комбинации" sheetId="43" r:id="rId8"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="191028"/>
@@ -256,19 +256,19 @@
     <x:t>11:30-11:45</x:t>
   </x:si>
   <x:si>
+    <x:t>10:15-10:30</x:t>
+  </x:si>
+  <x:si>
     <x:t>11:15-11:30</x:t>
   </x:si>
   <x:si>
-    <x:t>10:15-10:30</x:t>
-  </x:si>
-  <x:si>
     <x:t>11:00-11:15</x:t>
   </x:si>
   <x:si>
+    <x:t>10:30-10:45</x:t>
+  </x:si>
+  <x:si>
     <x:t>10:45-11:00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:30-10:45</x:t>
   </x:si>
   <x:si>
     <x:t>10:00-10:15</x:t>
@@ -1264,19 +1264,19 @@
         <x:v>77</x:v>
       </x:c>
       <x:c r="G1" s="12" t="s">
-        <x:v>73</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="H1" s="12" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="I1" s="12" t="s">
         <x:v>76</x:v>
-      </x:c>
-      <x:c r="I1" s="12" t="s">
-        <x:v>75</x:v>
       </x:c>
       <x:c r="J1" s="12" t="s">
         <x:v>74</x:v>
       </x:c>
       <x:c r="K1" s="12" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="L1" s="12" t="s">
         <x:v>71</x:v>

</xml_diff>

<commit_message>
Revert "start of transition to time slots"
This reverts commit 441ccb82877ec59f5b62480c6368b6912adf39f0.
</commit_message>
<xml_diff>
--- a/Shedule/Shedule/example.xlsx
+++ b/Shedule/Shedule/example.xlsx
@@ -16,7 +16,7 @@
     <x:sheet name="преподы" sheetId="2" r:id="rId1"/>
     <x:sheet name="ученики" sheetId="1" r:id="rId2"/>
     <x:sheet name="квалификации" sheetId="3" r:id="rId3"/>
-    <x:sheet name="Расписание и комбинации" sheetId="43" r:id="rId8"/>
+    <x:sheet name="Расписание и комбинации" sheetId="40" r:id="rId8"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="191028"/>
@@ -256,19 +256,19 @@
     <x:t>11:30-11:45</x:t>
   </x:si>
   <x:si>
+    <x:t>11:15-11:30</x:t>
+  </x:si>
+  <x:si>
     <x:t>10:15-10:30</x:t>
   </x:si>
   <x:si>
-    <x:t>11:15-11:30</x:t>
-  </x:si>
-  <x:si>
     <x:t>11:00-11:15</x:t>
   </x:si>
   <x:si>
+    <x:t>10:45-11:00</x:t>
+  </x:si>
+  <x:si>
     <x:t>10:30-10:45</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10:45-11:00</x:t>
   </x:si>
   <x:si>
     <x:t>10:00-10:15</x:t>
@@ -1264,19 +1264,19 @@
         <x:v>77</x:v>
       </x:c>
       <x:c r="G1" s="12" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="H1" s="12" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="I1" s="12" t="s">
         <x:v>75</x:v>
-      </x:c>
-      <x:c r="I1" s="12" t="s">
-        <x:v>76</x:v>
       </x:c>
       <x:c r="J1" s="12" t="s">
         <x:v>74</x:v>
       </x:c>
       <x:c r="K1" s="12" t="s">
-        <x:v>73</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="L1" s="12" t="s">
         <x:v>71</x:v>

</xml_diff>